<commit_message>
Updated xlsx file Updated functional_specs
Added code samples for MVC
Added EventType enum
</commit_message>
<xml_diff>
--- a/SplendorDoc/splendor_methods.xlsx
+++ b/SplendorDoc/splendor_methods.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Player</t>
   </si>
@@ -118,6 +117,9 @@
   </si>
   <si>
     <t>give_back_token</t>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
@@ -272,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -294,6 +296,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,6 +420,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -419,15 +436,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -448,6 +456,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -460,7 +536,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B3:G15" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6" headerRowCellStyle="Insatisfaisant" dataCellStyle="Insatisfaisant">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B3:G15" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B3:G15"/>
   <tableColumns count="6">
     <tableColumn id="1" name="GameRules (Controller)" dataDxfId="5"/>
@@ -479,7 +555,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="464646"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -740,7 +816,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,8 +891,12 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>7</v>
@@ -872,7 +952,9 @@
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -902,7 +984,9 @@
       <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>

</xml_diff>